<commit_message>
Jackie added comments to sorting algorithms. I added the dependencies for Apache POI to a lib folder.
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="13">
   <si>
     <t>Pass</t>
   </si>
@@ -2806,7 +2806,7 @@
         <v>1000.0</v>
       </c>
       <c r="C2" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -2820,7 +2820,7 @@
         <v>10000.0</v>
       </c>
       <c r="C3" t="n">
-        <v>150.0</v>
+        <v>149.0</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -2834,7 +2834,7 @@
         <v>100000.0</v>
       </c>
       <c r="C4" t="n">
-        <v>14007.0</v>
+        <v>13191.0</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
@@ -2862,7 +2862,7 @@
         <v>10000.0</v>
       </c>
       <c r="C6" t="n">
-        <v>120.0</v>
+        <v>121.0</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
@@ -2876,7 +2876,7 @@
         <v>100000.0</v>
       </c>
       <c r="C7" t="n">
-        <v>14105.0</v>
+        <v>13209.0</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -2890,7 +2890,7 @@
         <v>1000.0</v>
       </c>
       <c r="C8" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
@@ -2904,7 +2904,7 @@
         <v>10000.0</v>
       </c>
       <c r="C9" t="n">
-        <v>119.0</v>
+        <v>120.0</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
@@ -2918,7 +2918,7 @@
         <v>100000.0</v>
       </c>
       <c r="C10" t="n">
-        <v>13963.0</v>
+        <v>13205.0</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
@@ -2946,7 +2946,7 @@
         <v>10000.0</v>
       </c>
       <c r="C12" t="n">
-        <v>120.0</v>
+        <v>121.0</v>
       </c>
       <c r="D12" t="s">
         <v>4</v>
@@ -2960,7 +2960,7 @@
         <v>100000.0</v>
       </c>
       <c r="C13" t="n">
-        <v>13969.0</v>
+        <v>13173.0</v>
       </c>
       <c r="D13" t="s">
         <v>4</v>
@@ -2988,7 +2988,7 @@
         <v>10000.0</v>
       </c>
       <c r="C15" t="n">
-        <v>120.0</v>
+        <v>121.0</v>
       </c>
       <c r="D15" t="s">
         <v>4</v>
@@ -3002,7 +3002,7 @@
         <v>100000.0</v>
       </c>
       <c r="C16" t="n">
-        <v>13966.0</v>
+        <v>13270.0</v>
       </c>
       <c r="D16" t="s">
         <v>4</v>
@@ -3030,7 +3030,7 @@
         <v>10000.0</v>
       </c>
       <c r="C18" t="n">
-        <v>119.0</v>
+        <v>122.0</v>
       </c>
       <c r="D18" t="s">
         <v>4</v>
@@ -3044,7 +3044,7 @@
         <v>100000.0</v>
       </c>
       <c r="C19" t="n">
-        <v>13922.0</v>
+        <v>13352.0</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
@@ -3058,7 +3058,7 @@
         <v>1000.0</v>
       </c>
       <c r="C20" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D20" t="s">
         <v>4</v>
@@ -3072,7 +3072,7 @@
         <v>10000.0</v>
       </c>
       <c r="C21" t="n">
-        <v>118.0</v>
+        <v>121.0</v>
       </c>
       <c r="D21" t="s">
         <v>4</v>
@@ -3086,7 +3086,7 @@
         <v>100000.0</v>
       </c>
       <c r="C22" t="n">
-        <v>13922.0</v>
+        <v>13462.0</v>
       </c>
       <c r="D22" t="s">
         <v>4</v>
@@ -3100,7 +3100,7 @@
         <v>1000.0</v>
       </c>
       <c r="C23" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D23" t="s">
         <v>4</v>
@@ -3128,7 +3128,7 @@
         <v>100000.0</v>
       </c>
       <c r="C25" t="n">
-        <v>14075.0</v>
+        <v>13314.0</v>
       </c>
       <c r="D25" t="s">
         <v>4</v>
@@ -3142,7 +3142,7 @@
         <v>1000.0</v>
       </c>
       <c r="C26" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D26" t="s">
         <v>4</v>
@@ -3156,7 +3156,7 @@
         <v>10000.0</v>
       </c>
       <c r="C27" t="n">
-        <v>120.0</v>
+        <v>124.0</v>
       </c>
       <c r="D27" t="s">
         <v>4</v>
@@ -3170,7 +3170,7 @@
         <v>100000.0</v>
       </c>
       <c r="C28" t="n">
-        <v>14091.0</v>
+        <v>13405.0</v>
       </c>
       <c r="D28" t="s">
         <v>4</v>
@@ -3184,7 +3184,7 @@
         <v>1000.0</v>
       </c>
       <c r="C29" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D29" t="s">
         <v>4</v>
@@ -3198,7 +3198,7 @@
         <v>10000.0</v>
       </c>
       <c r="C30" t="n">
-        <v>120.0</v>
+        <v>122.0</v>
       </c>
       <c r="D30" t="s">
         <v>4</v>
@@ -3212,7 +3212,7 @@
         <v>100000.0</v>
       </c>
       <c r="C31" t="n">
-        <v>14303.0</v>
+        <v>13289.0</v>
       </c>
       <c r="D31" t="s">
         <v>4</v>
@@ -3285,7 +3285,7 @@
         <v>100000.0</v>
       </c>
       <c r="C4" t="n">
-        <v>4080.0</v>
+        <v>4089.0</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
@@ -3327,7 +3327,7 @@
         <v>100000.0</v>
       </c>
       <c r="C7" t="n">
-        <v>4086.0</v>
+        <v>4070.0</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -3369,7 +3369,7 @@
         <v>100000.0</v>
       </c>
       <c r="C10" t="n">
-        <v>4066.0</v>
+        <v>4068.0</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
@@ -3411,7 +3411,7 @@
         <v>100000.0</v>
       </c>
       <c r="C13" t="n">
-        <v>4072.0</v>
+        <v>4074.0</v>
       </c>
       <c r="D13" t="s">
         <v>4</v>
@@ -3453,7 +3453,7 @@
         <v>100000.0</v>
       </c>
       <c r="C16" t="n">
-        <v>4351.0</v>
+        <v>4063.0</v>
       </c>
       <c r="D16" t="s">
         <v>4</v>
@@ -3495,7 +3495,7 @@
         <v>100000.0</v>
       </c>
       <c r="C19" t="n">
-        <v>4167.0</v>
+        <v>4063.0</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
@@ -3523,7 +3523,7 @@
         <v>10000.0</v>
       </c>
       <c r="C21" t="n">
-        <v>47.0</v>
+        <v>41.0</v>
       </c>
       <c r="D21" t="s">
         <v>4</v>
@@ -3537,7 +3537,7 @@
         <v>100000.0</v>
       </c>
       <c r="C22" t="n">
-        <v>4140.0</v>
+        <v>4061.0</v>
       </c>
       <c r="D22" t="s">
         <v>4</v>
@@ -3565,7 +3565,7 @@
         <v>10000.0</v>
       </c>
       <c r="C24" t="n">
-        <v>45.0</v>
+        <v>41.0</v>
       </c>
       <c r="D24" t="s">
         <v>4</v>
@@ -3579,7 +3579,7 @@
         <v>100000.0</v>
       </c>
       <c r="C25" t="n">
-        <v>4078.0</v>
+        <v>4060.0</v>
       </c>
       <c r="D25" t="s">
         <v>4</v>
@@ -3621,7 +3621,7 @@
         <v>100000.0</v>
       </c>
       <c r="C28" t="n">
-        <v>4176.0</v>
+        <v>4061.0</v>
       </c>
       <c r="D28" t="s">
         <v>4</v>
@@ -3663,7 +3663,7 @@
         <v>100000.0</v>
       </c>
       <c r="C31" t="n">
-        <v>4082.0</v>
+        <v>4058.0</v>
       </c>
       <c r="D31" t="s">
         <v>4</v>
@@ -3735,7 +3735,7 @@
         <v>100000.0</v>
       </c>
       <c r="C4" t="n">
-        <v>1321.0</v>
+        <v>1324.0</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
@@ -3763,7 +3763,7 @@
         <v>10000.0</v>
       </c>
       <c r="C6" t="n">
-        <v>13.0</v>
+        <v>18.0</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
@@ -3777,7 +3777,7 @@
         <v>100000.0</v>
       </c>
       <c r="C7" t="n">
-        <v>1321.0</v>
+        <v>1322.0</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -3819,7 +3819,7 @@
         <v>100000.0</v>
       </c>
       <c r="C10" t="n">
-        <v>1320.0</v>
+        <v>1315.0</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
@@ -3861,7 +3861,7 @@
         <v>100000.0</v>
       </c>
       <c r="C13" t="n">
-        <v>1318.0</v>
+        <v>1316.0</v>
       </c>
       <c r="D13" t="s">
         <v>4</v>
@@ -3945,7 +3945,7 @@
         <v>100000.0</v>
       </c>
       <c r="C19" t="n">
-        <v>1316.0</v>
+        <v>1322.0</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
@@ -3987,7 +3987,7 @@
         <v>100000.0</v>
       </c>
       <c r="C22" t="n">
-        <v>1316.0</v>
+        <v>1323.0</v>
       </c>
       <c r="D22" t="s">
         <v>4</v>
@@ -4029,7 +4029,7 @@
         <v>100000.0</v>
       </c>
       <c r="C25" t="n">
-        <v>1317.0</v>
+        <v>1318.0</v>
       </c>
       <c r="D25" t="s">
         <v>4</v>
@@ -4071,7 +4071,7 @@
         <v>100000.0</v>
       </c>
       <c r="C28" t="n">
-        <v>1321.0</v>
+        <v>1316.0</v>
       </c>
       <c r="D28" t="s">
         <v>4</v>
@@ -4113,7 +4113,7 @@
         <v>100000.0</v>
       </c>
       <c r="C31" t="n">
-        <v>1315.0</v>
+        <v>1327.0</v>
       </c>
       <c r="D31" t="s">
         <v>4</v>
@@ -4199,7 +4199,7 @@
         <v>1000000.0</v>
       </c>
       <c r="C5" t="n">
-        <v>116.0</v>
+        <v>113.0</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
@@ -4213,7 +4213,7 @@
         <v>2000000.0</v>
       </c>
       <c r="C6" t="n">
-        <v>238.0</v>
+        <v>234.0</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
@@ -4255,7 +4255,7 @@
         <v>100000.0</v>
       </c>
       <c r="C9" t="n">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
@@ -4283,7 +4283,7 @@
         <v>2000000.0</v>
       </c>
       <c r="C11" t="n">
-        <v>237.0</v>
+        <v>232.0</v>
       </c>
       <c r="D11" t="s">
         <v>4</v>
@@ -4339,7 +4339,7 @@
         <v>1000000.0</v>
       </c>
       <c r="C15" t="n">
-        <v>133.0</v>
+        <v>114.0</v>
       </c>
       <c r="D15" t="s">
         <v>4</v>
@@ -4353,7 +4353,7 @@
         <v>2000000.0</v>
       </c>
       <c r="C16" t="n">
-        <v>233.0</v>
+        <v>236.0</v>
       </c>
       <c r="D16" t="s">
         <v>4</v>
@@ -4395,7 +4395,7 @@
         <v>100000.0</v>
       </c>
       <c r="C19" t="n">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
@@ -4409,7 +4409,7 @@
         <v>1000000.0</v>
       </c>
       <c r="C20" t="n">
-        <v>115.0</v>
+        <v>114.0</v>
       </c>
       <c r="D20" t="s">
         <v>4</v>
@@ -4423,7 +4423,7 @@
         <v>2000000.0</v>
       </c>
       <c r="C21" t="n">
-        <v>235.0</v>
+        <v>233.0</v>
       </c>
       <c r="D21" t="s">
         <v>4</v>
@@ -4479,7 +4479,7 @@
         <v>1000000.0</v>
       </c>
       <c r="C25" t="n">
-        <v>114.0</v>
+        <v>113.0</v>
       </c>
       <c r="D25" t="s">
         <v>4</v>
@@ -4493,7 +4493,7 @@
         <v>2000000.0</v>
       </c>
       <c r="C26" t="n">
-        <v>233.0</v>
+        <v>234.0</v>
       </c>
       <c r="D26" t="s">
         <v>4</v>
@@ -4535,7 +4535,7 @@
         <v>100000.0</v>
       </c>
       <c r="C29" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="D29" t="s">
         <v>4</v>
@@ -4549,7 +4549,7 @@
         <v>1000000.0</v>
       </c>
       <c r="C30" t="n">
-        <v>115.0</v>
+        <v>113.0</v>
       </c>
       <c r="D30" t="s">
         <v>4</v>
@@ -4563,7 +4563,7 @@
         <v>2000000.0</v>
       </c>
       <c r="C31" t="n">
-        <v>233.0</v>
+        <v>234.0</v>
       </c>
       <c r="D31" t="s">
         <v>4</v>
@@ -4605,7 +4605,7 @@
         <v>100000.0</v>
       </c>
       <c r="C34" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="D34" t="s">
         <v>4</v>
@@ -4619,7 +4619,7 @@
         <v>1000000.0</v>
       </c>
       <c r="C35" t="n">
-        <v>115.0</v>
+        <v>113.0</v>
       </c>
       <c r="D35" t="s">
         <v>4</v>
@@ -4633,7 +4633,7 @@
         <v>2000000.0</v>
       </c>
       <c r="C36" t="n">
-        <v>235.0</v>
+        <v>234.0</v>
       </c>
       <c r="D36" t="s">
         <v>4</v>
@@ -4675,7 +4675,7 @@
         <v>100000.0</v>
       </c>
       <c r="C39" t="n">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="D39" t="s">
         <v>4</v>
@@ -4703,7 +4703,7 @@
         <v>2000000.0</v>
       </c>
       <c r="C41" t="n">
-        <v>235.0</v>
+        <v>234.0</v>
       </c>
       <c r="D41" t="s">
         <v>4</v>
@@ -4759,7 +4759,7 @@
         <v>1000000.0</v>
       </c>
       <c r="C45" t="n">
-        <v>114.0</v>
+        <v>113.0</v>
       </c>
       <c r="D45" t="s">
         <v>4</v>
@@ -4773,7 +4773,7 @@
         <v>2000000.0</v>
       </c>
       <c r="C46" t="n">
-        <v>236.0</v>
+        <v>230.0</v>
       </c>
       <c r="D46" t="s">
         <v>4</v>
@@ -4829,7 +4829,7 @@
         <v>1000000.0</v>
       </c>
       <c r="C50" t="n">
-        <v>116.0</v>
+        <v>114.0</v>
       </c>
       <c r="D50" t="s">
         <v>4</v>
@@ -4843,7 +4843,7 @@
         <v>2000000.0</v>
       </c>
       <c r="C51" t="n">
-        <v>235.0</v>
+        <v>232.0</v>
       </c>
       <c r="D51" t="s">
         <v>4</v>
@@ -4915,7 +4915,7 @@
         <v>100000.0</v>
       </c>
       <c r="C4" t="n">
-        <v>19.0</v>
+        <v>21.0</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
@@ -4929,7 +4929,7 @@
         <v>1000000.0</v>
       </c>
       <c r="C5" t="n">
-        <v>187.0</v>
+        <v>194.0</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
@@ -4943,7 +4943,7 @@
         <v>2000000.0</v>
       </c>
       <c r="C6" t="n">
-        <v>393.0</v>
+        <v>432.0</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
@@ -4999,7 +4999,7 @@
         <v>1000000.0</v>
       </c>
       <c r="C10" t="n">
-        <v>186.0</v>
+        <v>201.0</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
@@ -5013,7 +5013,7 @@
         <v>2000000.0</v>
       </c>
       <c r="C11" t="n">
-        <v>377.0</v>
+        <v>421.0</v>
       </c>
       <c r="D11" t="s">
         <v>4</v>
@@ -5055,7 +5055,7 @@
         <v>100000.0</v>
       </c>
       <c r="C14" t="n">
-        <v>16.0</v>
+        <v>14.0</v>
       </c>
       <c r="D14" t="s">
         <v>4</v>
@@ -5069,7 +5069,7 @@
         <v>1000000.0</v>
       </c>
       <c r="C15" t="n">
-        <v>173.0</v>
+        <v>175.0</v>
       </c>
       <c r="D15" t="s">
         <v>4</v>
@@ -5083,7 +5083,7 @@
         <v>2000000.0</v>
       </c>
       <c r="C16" t="n">
-        <v>397.0</v>
+        <v>453.0</v>
       </c>
       <c r="D16" t="s">
         <v>4</v>
@@ -5125,7 +5125,7 @@
         <v>100000.0</v>
       </c>
       <c r="C19" t="n">
-        <v>17.0</v>
+        <v>21.0</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
@@ -5139,7 +5139,7 @@
         <v>1000000.0</v>
       </c>
       <c r="C20" t="n">
-        <v>181.0</v>
+        <v>204.0</v>
       </c>
       <c r="D20" t="s">
         <v>4</v>
@@ -5209,7 +5209,7 @@
         <v>1000000.0</v>
       </c>
       <c r="C25" t="n">
-        <v>176.0</v>
+        <v>180.0</v>
       </c>
       <c r="D25" t="s">
         <v>4</v>
@@ -5223,7 +5223,7 @@
         <v>2000000.0</v>
       </c>
       <c r="C26" t="n">
-        <v>359.0</v>
+        <v>358.0</v>
       </c>
       <c r="D26" t="s">
         <v>4</v>
@@ -5279,7 +5279,7 @@
         <v>1000000.0</v>
       </c>
       <c r="C30" t="n">
-        <v>181.0</v>
+        <v>185.0</v>
       </c>
       <c r="D30" t="s">
         <v>4</v>
@@ -5293,7 +5293,7 @@
         <v>2000000.0</v>
       </c>
       <c r="C31" t="n">
-        <v>418.0</v>
+        <v>511.0</v>
       </c>
       <c r="D31" t="s">
         <v>4</v>
@@ -5349,7 +5349,7 @@
         <v>1000000.0</v>
       </c>
       <c r="C35" t="n">
-        <v>172.0</v>
+        <v>173.0</v>
       </c>
       <c r="D35" t="s">
         <v>4</v>
@@ -5433,7 +5433,7 @@
         <v>2000000.0</v>
       </c>
       <c r="C41" t="n">
-        <v>365.0</v>
+        <v>369.0</v>
       </c>
       <c r="D41" t="s">
         <v>4</v>
@@ -5489,7 +5489,7 @@
         <v>1000000.0</v>
       </c>
       <c r="C45" t="n">
-        <v>172.0</v>
+        <v>173.0</v>
       </c>
       <c r="D45" t="s">
         <v>4</v>
@@ -5503,7 +5503,7 @@
         <v>2000000.0</v>
       </c>
       <c r="C46" t="n">
-        <v>357.0</v>
+        <v>358.0</v>
       </c>
       <c r="D46" t="s">
         <v>4</v>
@@ -5545,7 +5545,7 @@
         <v>100000.0</v>
       </c>
       <c r="C49" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
       <c r="D49" t="s">
         <v>4</v>
@@ -5559,7 +5559,7 @@
         <v>1000000.0</v>
       </c>
       <c r="C50" t="n">
-        <v>173.0</v>
+        <v>174.0</v>
       </c>
       <c r="D50" t="s">
         <v>4</v>
@@ -5573,7 +5573,7 @@
         <v>2000000.0</v>
       </c>
       <c r="C51" t="n">
-        <v>415.0</v>
+        <v>447.0</v>
       </c>
       <c r="D51" t="s">
         <v>4</v>

</xml_diff>